<commit_message>
tung - 5 // Add file python for process audio
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK9\doAnChuyenNganhNhung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK9\doAnChuyenNganhNhung\code\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>url</t>
   </si>
@@ -90,6 +90,18 @@
       "_id": "5bb8e0d04df33705e4edf5e9"
     }
   ]}</t>
+  </si>
+  <si>
+    <t>./download/gape</t>
+  </si>
+  <si>
+    <t>./script/gape</t>
+  </si>
+  <si>
+    <t>load màn hình để upload thêm script</t>
+  </si>
+  <si>
+    <t>load màn hình để download dữ liệu</t>
   </si>
 </sst>
 </file>
@@ -124,13 +136,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,15 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="96.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -439,7 +455,7 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -453,7 +469,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
@@ -467,7 +483,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -478,7 +494,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -489,11 +505,33 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>